<commit_message>
jenkinksFile y Serenity propertis
</commit_message>
<xml_diff>
--- a/P-Geo/src/test/resources/dataDriven/LRETAMOZO/DataPrueba.xlsx
+++ b/P-Geo/src/test/resources/dataDriven/LRETAMOZO/DataPrueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_WS\Geolocalizacion\P-Geo\src\test\resources\dataDriven\LRETAMOZO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LRETAMOZO\git\GeolocalizacionJenkins\P-Geo\src\test\resources\dataDriven\LRETAMOZO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD37F289-F857-45B0-9EA6-5918D83C0A1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAF6F08-90A0-427D-8CFD-A1F8A2FD89B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01-RegistrarAtencion" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="42">
   <si>
     <t>usar</t>
   </si>
@@ -121,33 +121,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ABA250</t>
-  </si>
-  <si>
-    <t>ABA251</t>
-  </si>
-  <si>
-    <t>ABA252</t>
-  </si>
-  <si>
-    <t>ABA253</t>
-  </si>
-  <si>
-    <t>ABA254</t>
-  </si>
-  <si>
-    <t>ABA255</t>
-  </si>
-  <si>
-    <t>ABA256</t>
-  </si>
-  <si>
-    <t>ABA257</t>
-  </si>
-  <si>
-    <t>ABA258</t>
-  </si>
-  <si>
     <t>PROCURADOR AUTO1</t>
   </si>
   <si>
@@ -158,6 +131,33 @@
   </si>
   <si>
     <t>PROCURADOR AUTO4</t>
+  </si>
+  <si>
+    <t>ABA259</t>
+  </si>
+  <si>
+    <t>ABA260</t>
+  </si>
+  <si>
+    <t>ABA261</t>
+  </si>
+  <si>
+    <t>ABA262</t>
+  </si>
+  <si>
+    <t>ABA263</t>
+  </si>
+  <si>
+    <t>ABA264</t>
+  </si>
+  <si>
+    <t>ABA265</t>
+  </si>
+  <si>
+    <t>ABA266</t>
+  </si>
+  <si>
+    <t>ABA267</t>
   </si>
 </sst>
 </file>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMC10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,9 +665,6 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
@@ -675,7 +672,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -697,9 +694,6 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -707,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -729,9 +723,6 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
@@ -739,7 +730,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -761,9 +752,6 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
@@ -771,7 +759,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -793,9 +781,6 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -803,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
@@ -835,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -867,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
@@ -899,7 +884,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -931,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>19</v>
@@ -970,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAA0A67-BA6C-453E-9BA4-3083C2316444}">
   <dimension ref="A1:AMD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -1017,10 +1002,10 @@
       </c>
       <c r="D2" s="1" t="str">
         <f>'01-RegistrarAtencion'!D2</f>
-        <v>ABA250</v>
+        <v>ABA259</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -1038,10 +1023,10 @@
       </c>
       <c r="D3" s="1" t="str">
         <f>'01-RegistrarAtencion'!D3</f>
-        <v>ABA251</v>
+        <v>ABA260</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -1059,10 +1044,10 @@
       </c>
       <c r="D4" s="1" t="str">
         <f>'01-RegistrarAtencion'!D4</f>
-        <v>ABA252</v>
+        <v>ABA261</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -1080,10 +1065,10 @@
       </c>
       <c r="D5" s="1" t="str">
         <f>'01-RegistrarAtencion'!D5</f>
-        <v>ABA253</v>
+        <v>ABA262</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>

</xml_diff>